<commit_message>
changed data, notebook, and function. Converted cones_function() to be a GLM; more precise estimates
</commit_message>
<xml_diff>
--- a/waffle_totals.xlsx
+++ b/waffle_totals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacksonrudoff/Documents/Data Projects/Waffle Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C637B116-8433-DA4A-86FF-D50E0C048F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36C81EC-7703-AD42-9C1F-9B15305FA644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{EE2C9ECB-D291-AF45-A5CA-85547B78DA43}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15760" xr2:uid="{EE2C9ECB-D291-AF45-A5CA-85547B78DA43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="10">
   <si>
     <t>Day</t>
   </si>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C776A25-50FC-CB46-BD2D-6F53350A1A6E}">
-  <dimension ref="A1:D156"/>
+  <dimension ref="A1:D196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="A197" sqref="A197:XFD260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2156,6 +2156,446 @@
         <v>48</v>
       </c>
     </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>4</v>
+      </c>
+      <c r="B157">
+        <v>44</v>
+      </c>
+      <c r="C157">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>5</v>
+      </c>
+      <c r="B158">
+        <v>91</v>
+      </c>
+      <c r="C158">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>6</v>
+      </c>
+      <c r="B159">
+        <v>108</v>
+      </c>
+      <c r="C159">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>7</v>
+      </c>
+      <c r="B160">
+        <v>159</v>
+      </c>
+      <c r="C160">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>8</v>
+      </c>
+      <c r="B161">
+        <v>224</v>
+      </c>
+      <c r="C161">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>9</v>
+      </c>
+      <c r="B162">
+        <v>257</v>
+      </c>
+      <c r="C162">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>3</v>
+      </c>
+      <c r="B163">
+        <v>186</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>4</v>
+      </c>
+      <c r="B164">
+        <v>75</v>
+      </c>
+      <c r="C164">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165">
+        <v>47</v>
+      </c>
+      <c r="C165">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>6</v>
+      </c>
+      <c r="B166">
+        <v>78</v>
+      </c>
+      <c r="C166">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>7</v>
+      </c>
+      <c r="B167">
+        <v>143</v>
+      </c>
+      <c r="C167">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>8</v>
+      </c>
+      <c r="B168">
+        <v>217</v>
+      </c>
+      <c r="C168">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>9</v>
+      </c>
+      <c r="B169">
+        <v>139</v>
+      </c>
+      <c r="C169">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>3</v>
+      </c>
+      <c r="B170">
+        <v>94</v>
+      </c>
+      <c r="C170">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>4</v>
+      </c>
+      <c r="B171">
+        <v>72</v>
+      </c>
+      <c r="C171">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172">
+        <v>88</v>
+      </c>
+      <c r="C172">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>6</v>
+      </c>
+      <c r="B173">
+        <v>87</v>
+      </c>
+      <c r="C173">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>7</v>
+      </c>
+      <c r="B174">
+        <v>134</v>
+      </c>
+      <c r="C174">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>8</v>
+      </c>
+      <c r="B175">
+        <v>158</v>
+      </c>
+      <c r="C175">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>9</v>
+      </c>
+      <c r="B176">
+        <v>161</v>
+      </c>
+      <c r="C176">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>3</v>
+      </c>
+      <c r="B177">
+        <v>83</v>
+      </c>
+      <c r="C177">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>4</v>
+      </c>
+      <c r="B178">
+        <v>46</v>
+      </c>
+      <c r="C178">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>5</v>
+      </c>
+      <c r="B179">
+        <v>56</v>
+      </c>
+      <c r="C179">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>6</v>
+      </c>
+      <c r="B180">
+        <v>56</v>
+      </c>
+      <c r="C180">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>7</v>
+      </c>
+      <c r="B181">
+        <v>125</v>
+      </c>
+      <c r="C181">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>8</v>
+      </c>
+      <c r="B182">
+        <v>139</v>
+      </c>
+      <c r="C182">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>9</v>
+      </c>
+      <c r="B183">
+        <v>191</v>
+      </c>
+      <c r="C183">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>3</v>
+      </c>
+      <c r="B184">
+        <v>123</v>
+      </c>
+      <c r="C184">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>4</v>
+      </c>
+      <c r="B185">
+        <v>86</v>
+      </c>
+      <c r="C185">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>5</v>
+      </c>
+      <c r="B186">
+        <v>98</v>
+      </c>
+      <c r="C186">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>6</v>
+      </c>
+      <c r="B187">
+        <v>120</v>
+      </c>
+      <c r="C187">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>7</v>
+      </c>
+      <c r="B188">
+        <v>139</v>
+      </c>
+      <c r="C188">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>8</v>
+      </c>
+      <c r="B189">
+        <v>193</v>
+      </c>
+      <c r="C189">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>9</v>
+      </c>
+      <c r="B190">
+        <v>130</v>
+      </c>
+      <c r="C190">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>3</v>
+      </c>
+      <c r="B191">
+        <v>61</v>
+      </c>
+      <c r="C191">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>4</v>
+      </c>
+      <c r="B192">
+        <v>65</v>
+      </c>
+      <c r="C192">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>5</v>
+      </c>
+      <c r="B193">
+        <v>51</v>
+      </c>
+      <c r="C193">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>6</v>
+      </c>
+      <c r="B194">
+        <v>85</v>
+      </c>
+      <c r="C194">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>7</v>
+      </c>
+      <c r="B195">
+        <v>130</v>
+      </c>
+      <c r="C195">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>8</v>
+      </c>
+      <c r="B196">
+        <v>230</v>
+      </c>
+      <c r="C196">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>